<commit_message>
added sprint review protocol
</commit_message>
<xml_diff>
--- a/final_upload_ring_retrieve_simulator/protocols/Sprint_Review_Protocol_Sprint1.xlsx
+++ b/final_upload_ring_retrieve_simulator/protocols/Sprint_Review_Protocol_Sprint1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Georg\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dominik\Documents\FH_Technikum\SS_2021\IT-Prj\2d-Rpg\final_upload_ring_retrieve_simulator\protocols\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4B55BD8-C93C-4D9F-95C6-C1232298B97C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DEEC78A-E55B-49BB-892C-808FE2E7D9A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
+    <workbookView xWindow="3675" yWindow="2310" windowWidth="21600" windowHeight="11385" xr2:uid="{5C77D34F-34C3-4D2F-849C-09193AE86D67}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -392,17 +392,23 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -410,50 +416,44 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="22" fontId="2" fillId="4" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -771,47 +771,47 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7AE3C726-37E9-451B-9308-D99ECF6E7468}">
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" style="2" customWidth="1"/>
-    <col min="2" max="2" width="32.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="13.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.44140625" style="2"/>
-    <col min="8" max="8" width="34.5546875" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="11.44140625" style="2"/>
+    <col min="2" max="2" width="32.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="11.42578125" style="2"/>
+    <col min="8" max="8" width="34.5703125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="29" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="29"/>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-    </row>
-    <row r="3" spans="1:9" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+    </row>
+    <row r="3" spans="1:9" ht="27" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A3" s="5"/>
       <c r="B3" s="5"/>
       <c r="C3" s="5"/>
@@ -822,11 +822,11 @@
       <c r="H3" s="5"/>
       <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A4" s="26" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="27"/>
+      <c r="B4" s="15"/>
       <c r="C4" s="18">
         <v>1</v>
       </c>
@@ -835,123 +835,123 @@
       <c r="F4" s="18"/>
       <c r="G4" s="19"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15"/>
-      <c r="C5" s="30">
+      <c r="B5" s="17"/>
+      <c r="C5" s="20">
         <v>44306.875</v>
       </c>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="21"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+      <c r="D5" s="21"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="21"/>
+      <c r="G5" s="22"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="20">
+      <c r="B6" s="17"/>
+      <c r="C6" s="21">
         <v>2</v>
       </c>
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-      <c r="F6" s="20"/>
-      <c r="G6" s="21"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="15"/>
-      <c r="C7" s="22" t="s">
+      <c r="B7" s="17"/>
+      <c r="C7" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="24"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="15"/>
-      <c r="C8" s="24" t="s">
+      <c r="B8" s="17"/>
+      <c r="C8" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="24"/>
-      <c r="G8" s="25"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="24" t="s">
+      <c r="B9" s="17"/>
+      <c r="C9" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="25"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="15"/>
-      <c r="C10" s="24" t="s">
+      <c r="B10" s="17"/>
+      <c r="C10" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
-      <c r="F10" s="24"/>
-      <c r="G10" s="25"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="13"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15"/>
-      <c r="C11" s="10" t="s">
+      <c r="B11" s="17"/>
+      <c r="C11" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="1:9" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="16" t="s">
+      <c r="D11" s="25"/>
+      <c r="E11" s="25"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="26"/>
+    </row>
+    <row r="12" spans="1:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="17"/>
-      <c r="C12" s="12" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="13"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A14" s="28" t="s">
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="28"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B14" s="28"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-      <c r="G14" s="28"/>
-      <c r="H14" s="28"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>10</v>
       </c>
@@ -977,7 +977,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>1</v>
       </c>
@@ -1000,7 +1000,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="7"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>2</v>
       </c>
@@ -1023,7 +1023,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="7"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>3</v>
       </c>
@@ -1046,7 +1046,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="7"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>4</v>
       </c>
@@ -1069,7 +1069,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="7"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>5</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
         <v>6</v>
       </c>
@@ -1117,7 +1117,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="7"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
         <v>7</v>
       </c>
@@ -1132,7 +1132,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="7"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -1147,7 +1147,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="7"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -1162,7 +1162,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="7"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>16</v>
       </c>
@@ -1177,14 +1177,17 @@
       <c r="G25" s="4"/>
       <c r="H25" s="7"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <f>COUNT(A16:A25)</f>
         <v>7</v>
       </c>
       <c r="B26" s="6"/>
       <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
+      <c r="D26" s="6">
+        <f>SUM(D16:D25)</f>
+        <v>49</v>
+      </c>
       <c r="E26" s="6">
         <f>SUM(E16:E25)</f>
         <v>0</v>
@@ -1199,19 +1202,23 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="B30" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
         <v>21</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="C12:G12"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
     <mergeCell ref="A14:H14"/>
     <mergeCell ref="A1:I2"/>
     <mergeCell ref="C8:G8"/>
@@ -1228,10 +1235,6 @@
     <mergeCell ref="C6:G6"/>
     <mergeCell ref="C7:G7"/>
     <mergeCell ref="C11:G11"/>
-    <mergeCell ref="C12:G12"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>